<commit_message>
Update Time Complexities of Algorithms.xlsx
</commit_message>
<xml_diff>
--- a/My Notes/PDSA/Time Complexities of Algorithms.xlsx
+++ b/My Notes/PDSA/Time Complexities of Algorithms.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\IIT-M\Programming Data Structures and Algorithms Using Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Official\GitHub\IIT-M\My Notes\PDSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFAE6EA-B5DE-46AD-93D3-9CC19DEBD075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F9DB43E-BA75-4229-AE8E-E01EE866D9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5C42CCC7-008D-4AC4-95D9-90038B64D50F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>Anand Iyer</author>
   </authors>
   <commentList>
-    <comment ref="A24" authorId="0" shapeId="0" xr:uid="{FDF70D14-C93C-423D-9095-8E31DA495787}">
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{FDF70D14-C93C-423D-9095-8E31DA495787}">
       <text>
         <r>
           <rPr>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="110">
   <si>
     <t>Algorithm</t>
   </si>
@@ -163,10 +163,6 @@
     <t>T(V, E) = T(V, E) + O(V)</t>
   </si>
   <si>
-    <t>O((V + E)log V)
-O(V2)</t>
-  </si>
-  <si>
     <t>Binary/Fibonacci heap
 Simple array</t>
   </si>
@@ -226,149 +222,172 @@
 Use MoM for partitioning</t>
   </si>
   <si>
-    <t>O(n2)
+    <t>QuickSelect</t>
+  </si>
+  <si>
+    <t>T(n) = T(n/2) + O(n)</t>
+  </si>
+  <si>
+    <t>Uses MoM</t>
+  </si>
+  <si>
+    <t>Uses random pivot</t>
+  </si>
+  <si>
+    <t>FastSelect</t>
+  </si>
+  <si>
+    <t>Many duplicates in array</t>
+  </si>
+  <si>
+    <t>T(n) = T(3n/10) + T(7n/10) + O(n)</t>
+  </si>
+  <si>
+    <t>Array is sorted in reverse</t>
+  </si>
+  <si>
+    <t>T(n) &lt;= T(2n/3) + O(1)</t>
+  </si>
+  <si>
+    <t>O(logn)</t>
+  </si>
+  <si>
+    <t>Heapify(Heap)</t>
+  </si>
+  <si>
+    <t>Insert(Heap)</t>
+  </si>
+  <si>
+    <t>T(n) = O(logn)</t>
+  </si>
+  <si>
+    <t>Extract(Heap)</t>
+  </si>
+  <si>
+    <t>Delete(Heap)</t>
+  </si>
+  <si>
+    <t>Build(Heap)</t>
+  </si>
+  <si>
+    <t>T(n) = O(n)</t>
+  </si>
+  <si>
+    <t>T(n) = T(h) + O(1)</t>
+  </si>
+  <si>
+    <t>Insert(BST)</t>
+  </si>
+  <si>
+    <t>h = tree height</t>
+  </si>
+  <si>
+    <t>BST is empty</t>
+  </si>
+  <si>
+    <t>O(log n)</t>
+  </si>
+  <si>
+    <t>Tree is balanced</t>
+  </si>
+  <si>
+    <t>Tree is skewed</t>
+  </si>
+  <si>
+    <t>Delete(BST)</t>
+  </si>
+  <si>
+    <t>Node has no children</t>
+  </si>
+  <si>
+    <t>Search(BST)</t>
+  </si>
+  <si>
+    <t>Target is root</t>
+  </si>
+  <si>
+    <t>Traversal(BST)</t>
+  </si>
+  <si>
+    <t>T(n) = 3T(n/2) + O(n)</t>
+  </si>
+  <si>
+    <t>multiply two n-digit numbers</t>
+  </si>
+  <si>
+    <t>O(n^log3)</t>
+  </si>
+  <si>
+    <t>Karatsuba</t>
+  </si>
+  <si>
+    <t>Search(AVL)</t>
+  </si>
+  <si>
+    <t>n = number of nodes</t>
+  </si>
+  <si>
+    <t>Insert(AVL)</t>
+  </si>
+  <si>
+    <t>Delete(AVL)</t>
+  </si>
+  <si>
+    <t>Rotate(AVL)</t>
+  </si>
+  <si>
+    <t>Rebalance(AVL)</t>
+  </si>
+  <si>
+    <t>Interval Scheduling</t>
+  </si>
+  <si>
+    <t>T(n) = O(n^2)</t>
+  </si>
+  <si>
+    <t>n = number of jobs</t>
+  </si>
+  <si>
+    <t>Intervals are already sorted</t>
+  </si>
+  <si>
+    <t>Minimizing lateness</t>
+  </si>
+  <si>
+    <t>Huffman</t>
+  </si>
+  <si>
+    <t>n = number of symbols</t>
+  </si>
+  <si>
+    <t>amortized n heapify ops</t>
+  </si>
+  <si>
+    <t>O(n^2)
 O(nlogn)</t>
   </si>
   <si>
-    <t>QuickSelect</t>
-  </si>
-  <si>
-    <t>T(n) = T(n/2) + O(n)</t>
-  </si>
-  <si>
-    <t>Uses MoM</t>
-  </si>
-  <si>
-    <t>Uses random pivot</t>
-  </si>
-  <si>
-    <t>FastSelect</t>
-  </si>
-  <si>
-    <t>Many duplicates in array</t>
-  </si>
-  <si>
-    <t>T(n) = T(3n/10) + T(7n/10) + O(n)</t>
-  </si>
-  <si>
-    <t>Array is sorted in reverse</t>
-  </si>
-  <si>
-    <t>T(n) &lt;= T(2n/3) + O(1)</t>
-  </si>
-  <si>
-    <t>O(logn)</t>
-  </si>
-  <si>
-    <t>Heapify(Heap)</t>
-  </si>
-  <si>
-    <t>Insert(Heap)</t>
-  </si>
-  <si>
-    <t>T(n) = O(logn)</t>
-  </si>
-  <si>
-    <t>Extract(Heap)</t>
-  </si>
-  <si>
-    <t>Delete(Heap)</t>
-  </si>
-  <si>
-    <t>Build(Heap)</t>
-  </si>
-  <si>
-    <t>T(n) = O(n)</t>
-  </si>
-  <si>
-    <t>T(n) = T(h) + O(1)</t>
-  </si>
-  <si>
-    <t>Insert(BST)</t>
-  </si>
-  <si>
-    <t>h = tree height</t>
-  </si>
-  <si>
-    <t>BST is empty</t>
-  </si>
-  <si>
-    <t>O(log n)</t>
-  </si>
-  <si>
-    <t>Tree is balanced</t>
-  </si>
-  <si>
-    <t>Tree is skewed</t>
-  </si>
-  <si>
-    <t>Delete(BST)</t>
-  </si>
-  <si>
-    <t>Node has no children</t>
-  </si>
-  <si>
-    <t>Search(BST)</t>
-  </si>
-  <si>
-    <t>Target is root</t>
-  </si>
-  <si>
-    <t>Traversal(BST)</t>
-  </si>
-  <si>
-    <t>T(n) = 3T(n/2) + O(n)</t>
-  </si>
-  <si>
-    <t>multiply two n-digit numbers</t>
-  </si>
-  <si>
-    <t>O(n^log3)</t>
-  </si>
-  <si>
-    <t>Karatsuba</t>
-  </si>
-  <si>
-    <t>Search(AVL)</t>
-  </si>
-  <si>
-    <t>n = number of nodes</t>
-  </si>
-  <si>
-    <t>Insert(AVL)</t>
-  </si>
-  <si>
-    <t>Delete(AVL)</t>
-  </si>
-  <si>
-    <t>Rotate(AVL)</t>
-  </si>
-  <si>
-    <t>Rebalance(AVL)</t>
-  </si>
-  <si>
-    <t>Interval Scheduling</t>
-  </si>
-  <si>
-    <t>T(n) = O(n^2)</t>
-  </si>
-  <si>
-    <t>n = number of jobs</t>
-  </si>
-  <si>
-    <t>Intervals are already sorted</t>
-  </si>
-  <si>
-    <t>Minimizing lateness</t>
-  </si>
-  <si>
-    <t>Huffman</t>
-  </si>
-  <si>
-    <t>n = number of symbols</t>
-  </si>
-  <si>
-    <t>amortized n heapify ops</t>
+    <t>O(n^2)</t>
+  </si>
+  <si>
+    <t>O((V + E)log V)
+O(n^2)</t>
+  </si>
+  <si>
+    <t>O((V + E)log V)
+O(V^2)</t>
+  </si>
+  <si>
+    <t>Union-Find</t>
+  </si>
+  <si>
+    <t>same component nodes</t>
+  </si>
+  <si>
+    <t>O(V logV)</t>
+  </si>
+  <si>
+    <t>Sequence of Union-Find ops</t>
   </si>
 </sst>
 </file>
@@ -569,8 +588,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3AB3CEB8-4A06-4D92-9E25-4B7EFF70A215}" name="Table1" displayName="Table1" ref="A1:I33" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I33" xr:uid="{3AB3CEB8-4A06-4D92-9E25-4B7EFF70A215}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3AB3CEB8-4A06-4D92-9E25-4B7EFF70A215}" name="Table1" displayName="Table1" ref="A1:I34" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I34" xr:uid="{3AB3CEB8-4A06-4D92-9E25-4B7EFF70A215}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{7AF0A783-9403-4861-A946-6D4724F0BEE5}" name="Algorithm" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{24C49CDE-CEFE-414B-BAEA-0093EA27CFDE}" name="Recurrence relation" dataDxfId="7"/>
@@ -883,9 +902,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5892C8-CEFB-4EF2-A077-670A4997AB20}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -895,7 +916,7 @@
     <col min="4" max="4" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="14" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.28515625" style="2" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
@@ -906,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>4</v>
@@ -950,10 +971,10 @@
         <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>56</v>
+        <v>102</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -993,7 +1014,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -1016,16 +1037,16 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1045,13 +1066,13 @@
         <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>27</v>
@@ -1071,7 +1092,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>29</v>
@@ -1094,7 +1115,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>29</v>
@@ -1117,27 +1138,27 @@
         <v>29</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="H9" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>33</v>
@@ -1146,41 +1167,41 @@
         <v>29</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>35</v>
@@ -1189,79 +1210,82 @@
         <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="F12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="H12" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>24</v>
+        <v>108</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>3</v>
+        <v>108</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>62</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>23</v>
@@ -1270,21 +1294,24 @@
         <v>24</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>24</v>
+        <v>103</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>23</v>
@@ -1292,321 +1319,324 @@
       <c r="D16" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="E16" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>24</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>17</v>
@@ -1618,41 +1648,41 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>12</v>
@@ -1661,15 +1691,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>12</v>
@@ -1678,6 +1708,26 @@
         <v>12</v>
       </c>
       <c r="H33" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>